<commit_message>
Simulated data beam steering 30-70deg.
</commit_message>
<xml_diff>
--- a/matlab/experiment/27Aug/45deg/sim45deg1.xlsx
+++ b/matlab/experiment/27Aug/45deg/sim45deg1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\waltd\OneDrive\Documents\2021\semester2\thesis-2021\matlab\experiment\27Aug\45deg\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315F6208-56DE-42CA-ACED-82712B023778}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C1FEC2C-71C5-4E19-A614-EE1FAE3AD80B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{8808EF6B-BA98-4E0C-BE3B-A375396529B2}"/>
   </bookViews>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="13">
   <si>
     <t>E1</t>
   </si>
@@ -68,6 +68,18 @@
   </si>
   <si>
     <t>E6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Spacing </t>
+  </si>
+  <si>
+    <t>Phase</t>
+  </si>
+  <si>
+    <t>Amplitude</t>
+  </si>
+  <si>
+    <t>Fitness</t>
   </si>
 </sst>
 </file>
@@ -7492,16 +7504,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>312421</xdr:colOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>53341</xdr:rowOff>
+      <xdr:rowOff>30481</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>358141</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>162387</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>236219</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>171051</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7524,8 +7536,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5798821" y="53341"/>
-          <a:ext cx="3703320" cy="3218006"/>
+          <a:off x="6438900" y="30481"/>
+          <a:ext cx="4160519" cy="3615290"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7537,15 +7549,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>76199</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>100456</xdr:rowOff>
+      <xdr:rowOff>1396</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>9</xdr:col>
-      <xdr:colOff>224258</xdr:colOff>
-      <xdr:row>17</xdr:row>
-      <xdr:rowOff>160019</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>169000</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -7568,8 +7580,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="76199" y="100456"/>
-          <a:ext cx="5634459" cy="3168523"/>
+          <a:off x="0" y="1396"/>
+          <a:ext cx="6477000" cy="3642324"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7580,16 +7592,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>594360</xdr:colOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>502920</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>175260</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>22</xdr:col>
-      <xdr:colOff>342900</xdr:colOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>464820</xdr:colOff>
       <xdr:row>17</xdr:row>
-      <xdr:rowOff>76200</xdr:rowOff>
+      <xdr:rowOff>53340</xdr:rowOff>
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
@@ -7604,8 +7616,8 @@
       </xdr:nvSpPr>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="9738360" y="175260"/>
-          <a:ext cx="4015740" cy="3009900"/>
+          <a:off x="10866120" y="152400"/>
+          <a:ext cx="2400300" cy="3009900"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -7721,7 +7733,7 @@
         <a:p>
           <a:r>
             <a:rPr lang="en-ZA" sz="1100" baseline="0"/>
-            <a:t>8 deg from target</a:t>
+            <a:t>10 deg from target</a:t>
           </a:r>
           <a:endParaRPr lang="en-ZA" sz="1100"/>
         </a:p>
@@ -7732,15 +7744,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>144780</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>449580</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>160020</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7770,15 +7782,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>548640</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>243840</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>30480</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7808,15 +7820,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>320040</xdr:colOff>
-      <xdr:row>21</xdr:row>
-      <xdr:rowOff>53340</xdr:rowOff>
+      <xdr:colOff>137160</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>22</xdr:col>
-      <xdr:colOff>579120</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>45720</xdr:rowOff>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7846,15 +7858,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>121920</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>426720</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>129540</xdr:rowOff>
+      <xdr:colOff>396240</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>22860</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -7884,15 +7896,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>7</xdr:col>
-      <xdr:colOff>563880</xdr:colOff>
-      <xdr:row>36</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>43</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>15</xdr:col>
-      <xdr:colOff>259080</xdr:colOff>
-      <xdr:row>51</xdr:row>
-      <xdr:rowOff>160020</xdr:rowOff>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>58</xdr:row>
+      <xdr:rowOff>30480</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -8219,14 +8231,89 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7A1A7E06-4BF8-438A-B8AD-9D6FC126E4B1}">
-  <dimension ref="A1"/>
+  <dimension ref="C22:I25"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="T42" sqref="T42"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K25" sqref="K25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData/>
+  <sheetData>
+    <row r="22" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C22" t="s">
+        <v>9</v>
+      </c>
+      <c r="D22">
+        <v>0.40600000000000003</v>
+      </c>
+      <c r="E22">
+        <v>0.502</v>
+      </c>
+      <c r="F22">
+        <v>0.64100000000000001</v>
+      </c>
+      <c r="G22">
+        <v>0.502</v>
+      </c>
+      <c r="H22">
+        <v>0.40600000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C23" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23">
+        <v>327.7</v>
+      </c>
+      <c r="E23">
+        <v>227.3</v>
+      </c>
+      <c r="F23">
+        <v>82.6</v>
+      </c>
+      <c r="G23">
+        <v>300</v>
+      </c>
+      <c r="H23">
+        <v>183.4</v>
+      </c>
+      <c r="I23">
+        <v>45.8</v>
+      </c>
+    </row>
+    <row r="24" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C24" t="s">
+        <v>11</v>
+      </c>
+      <c r="D24">
+        <v>0.58899999999999997</v>
+      </c>
+      <c r="E24">
+        <v>0.85699999999999998</v>
+      </c>
+      <c r="F24">
+        <v>0.92700000000000005</v>
+      </c>
+      <c r="G24">
+        <v>0.47099999999999997</v>
+      </c>
+      <c r="H24">
+        <v>0.83199999999999996</v>
+      </c>
+      <c r="I24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="3:9" x14ac:dyDescent="0.3">
+      <c r="C25" t="s">
+        <v>12</v>
+      </c>
+      <c r="D25">
+        <v>-4.3752818042035457</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -8236,8 +8323,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6AC0843D-02D6-4029-B1B8-71B6557E84A8}">
   <dimension ref="A1:E51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:E51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9112,8 +9199,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E54983D9-4BB8-4744-9DA2-979A017FCC8C}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:XFD1"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -10147,8 +10234,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1DFE3960-CEC6-442D-9643-620A0968C7FF}">
   <dimension ref="A1:F51"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1048576"/>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A51" sqref="A51:F51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -11713,7 +11800,7 @@
   <dimension ref="A1:A50"/>
   <sheetViews>
     <sheetView topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A18" sqref="A1:A1048576"/>
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>